<commit_message>
added backgroundcolor to table header ad notification sheet
</commit_message>
<xml_diff>
--- a/勤怠報告書（2021年度_大野原信）.xlsx
+++ b/勤怠報告書（2021年度_大野原信）.xlsx
@@ -152,7 +152,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="ＭＳ ゴシック"/>
+      <name val="Calibri"/>
       <sz val="11.0"/>
     </font>
     <font>
@@ -214,12 +214,22 @@
       <color indexed="10"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="CCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="CCFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
@@ -284,13 +294,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -318,22 +328,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyAlignment="true" applyFont="true" applyFill="true">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyAlignment="true" applyFont="true" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyAlignment="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyAlignment="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyAlignment="true" applyFill="true" applyFont="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyAlignment="true" applyFont="true" applyFill="true" applyBorder="true">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyAlignment="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyAlignment="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyAlignment="true" applyFont="true" applyFill="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyAlignment="true" applyFont="true" applyFill="true" applyBorder="true">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyAlignment="true" applyFont="true" applyFill="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1081,11 +1091,18 @@
       <c r="L48"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="12">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
     <mergeCell ref="A48:L48"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>